<commit_message>
Further calibrate bldgs/SoCEUtiNTY and trans/SoCDTtiNTY
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1411,10 +1411,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1733,17 +1733,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1751,167 +1751,167 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="30" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B17" s="30" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B19" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B24" s="30" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B25" s="33" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>379</v>
       </c>
@@ -1928,13 +1928,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>15.833333333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>51.81818181818182</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>9.1324200913242013</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>13.533333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2006,14 +2006,14 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="6"/>
+    <col min="1" max="1" width="19.86328125" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="43.59765625" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="8.73046875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="21" t="s">
         <v>181</v>
       </c>
@@ -2126,8 +2126,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="23" t="s">
         <v>180</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="23" t="s">
         <v>178</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="23" t="s">
         <v>175</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="23" t="s">
         <v>173</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="11" t="s">
         <v>339</v>
       </c>
@@ -2181,12 +2181,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
         <v>168</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="19" t="s">
         <v>166</v>
       </c>
@@ -2418,18 +2418,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>336</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>8.4399999999999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>334</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>1.0499E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>332</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>-7.2430000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>330</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>8.3569999999999998E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>329</v>
       </c>
@@ -3024,17 +3024,17 @@
         <v>3.7309999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="10" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>325</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>-7.7879999999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>324</v>
       </c>
@@ -3272,12 +3272,12 @@
         <v>-8.8489999999999992E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>323</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>-1.1476E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>321</v>
       </c>
@@ -3515,17 +3515,17 @@
         <v>-1.2533000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>319</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>-1.041E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>318</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>6.9200000000000002E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>317</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>1.9040000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>316</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>3.362E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>315</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>1.0992999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>314</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>8.9499999999999996E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>313</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>-2.4559999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>311</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>-1.7500999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>310</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>-9.953E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>308</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>1.2205000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="11" t="s">
         <v>306</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>5.1910000000000003E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>304</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>-3.2238000000000003E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
         <v>302</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>-2.0820000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="11" t="s">
         <v>300</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>6.9309999999999997E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>299</v>
       </c>
@@ -5310,12 +5310,12 @@
         <v>2.2339999999999999E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="11" t="s">
         <v>298</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>2.9799999999999998E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="11" t="s">
         <v>297</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>-7.4190000000000002E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="11" t="s">
         <v>295</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>2.3839999999999998E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="11" t="s">
         <v>294</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>3.7450000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="11" t="s">
         <v>293</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>6.659E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="11" t="s">
         <v>291</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>-5.071E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
         <v>289</v>
       </c>
@@ -6148,12 +6148,12 @@
         <v>8.1099999999999998E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="11" t="s">
         <v>288</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>-1.4128E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="11" t="s">
         <v>287</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>-3.7629999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="11" t="s">
         <v>286</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>-6.2040000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>285</v>
       </c>
@@ -6629,12 +6629,12 @@
         <v>-1.5632E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="11" t="s">
         <v>283</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>-7.0309999999999999E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="11" t="s">
         <v>281</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>-1.7628999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="11" t="s">
         <v>279</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>-5.5599999999999998E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="11" t="s">
         <v>278</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>1.4448000000000001E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
         <v>277</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>-4.9649999999999998E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="11" t="s">
         <v>276</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>-6.3109999999999998E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="11" t="s">
         <v>274</v>
       </c>
@@ -7467,12 +7467,12 @@
         <v>-2.0202999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="11" t="s">
         <v>272</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>-1.9480000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="11" t="s">
         <v>271</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>4.9600000000000002E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="11" t="s">
         <v>270</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>1.214E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="11" t="s">
         <v>269</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>3.362E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="11" t="s">
         <v>268</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="11" t="s">
         <v>267</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>8.5059999999999997E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="11" t="s">
         <v>266</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>-2.4559999999999998E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="11" t="s">
         <v>265</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>-1.7500999999999999E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="11" t="s">
         <v>264</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>-9.953E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="11" t="s">
         <v>263</v>
       </c>
@@ -8662,7 +8662,7 @@
         <v>1.2205000000000001E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="11" t="s">
         <v>262</v>
       </c>
@@ -8781,7 +8781,7 @@
         <v>5.1910000000000003E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="11" t="s">
         <v>261</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>-3.2238000000000003E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="11" t="s">
         <v>260</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>-2.0820000000000001E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="11" t="s">
         <v>259</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>5.6210000000000001E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="11" t="s">
         <v>258</v>
       </c>
@@ -9257,7 +9257,7 @@
         <v>5.04E-4</v>
       </c>
     </row>
-    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="11" t="s">
         <v>256</v>
       </c>
@@ -9376,12 +9376,12 @@
         <v>-1.823E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="11" t="s">
         <v>255</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>-2.343E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="11" t="s">
         <v>253</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>-1.9719999999999998E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="11" t="s">
         <v>251</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
     </row>
-    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="11" t="s">
         <v>249</v>
       </c>
@@ -9857,7 +9857,7 @@
         <v>7.3899999999999997E-4</v>
       </c>
     </row>
-    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="11" t="s">
         <v>247</v>
       </c>
@@ -9976,7 +9976,7 @@
         <v>6.1139999999999996E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="11" t="s">
         <v>245</v>
       </c>
@@ -10095,7 +10095,7 @@
         <v>6.339E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="11" t="s">
         <v>243</v>
       </c>
@@ -10214,7 +10214,7 @@
         <v>-5.0639999999999999E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="11" t="s">
         <v>241</v>
       </c>
@@ -10333,7 +10333,7 @@
         <v>-2.0070000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="11" t="s">
         <v>239</v>
       </c>
@@ -10452,7 +10452,7 @@
         <v>-1.2541999999999999E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="11" t="s">
         <v>237</v>
       </c>
@@ -10571,7 +10571,7 @@
         <v>9.5589999999999998E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="11" t="s">
         <v>235</v>
       </c>
@@ -10690,7 +10690,7 @@
         <v>2.562E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="11" t="s">
         <v>233</v>
       </c>
@@ -10809,7 +10809,7 @@
         <v>-3.4768E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="11" t="s">
         <v>231</v>
       </c>
@@ -10928,7 +10928,7 @@
         <v>-4.6909999999999999E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="11" t="s">
         <v>229</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>3.9480000000000001E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="11" t="s">
         <v>227</v>
       </c>
@@ -11166,12 +11166,12 @@
         <v>-5.6499999999999996E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="10" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="11" t="s">
         <v>224</v>
       </c>
@@ -11290,7 +11290,7 @@
         <v>2.7342999999999999E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="11" t="s">
         <v>222</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>2.7820999999999999E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="11" t="s">
         <v>220</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>9.7493999999999997E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="11" t="s">
         <v>219</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>9.724E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="11" t="s">
         <v>218</v>
       </c>
@@ -11766,12 +11766,12 @@
         <v>8.5554000000000005E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B118" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="11" t="s">
         <v>217</v>
       </c>
@@ -11890,7 +11890,7 @@
         <v>-1.8090000000000001E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120" s="11" t="s">
         <v>216</v>
       </c>
@@ -12009,7 +12009,7 @@
         <v>-1.7240000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121" s="11" t="s">
         <v>215</v>
       </c>
@@ -12128,7 +12128,7 @@
         <v>1.0460000000000001E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122" s="11" t="s">
         <v>214</v>
       </c>
@@ -12247,7 +12247,7 @@
         <v>1.934E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123" s="11" t="s">
         <v>213</v>
       </c>
@@ -12366,7 +12366,7 @@
         <v>-2.6310000000000001E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124" s="11" t="s">
         <v>212</v>
       </c>
@@ -12485,7 +12485,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
     </row>
-    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125" s="11" t="s">
         <v>211</v>
       </c>
@@ -12604,7 +12604,7 @@
         <v>1.5E-5</v>
       </c>
     </row>
-    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126" s="11" t="s">
         <v>210</v>
       </c>
@@ -12723,7 +12723,7 @@
         <v>-9.4700000000000003E-4</v>
       </c>
     </row>
-    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127" s="11" t="s">
         <v>209</v>
       </c>
@@ -12842,7 +12842,7 @@
         <v>1.7769999999999999E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="11" t="s">
         <v>208</v>
       </c>
@@ -12961,12 +12961,12 @@
         <v>-1.3990000000000001E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B130" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131" s="11" t="s">
         <v>207</v>
       </c>
@@ -13085,7 +13085,7 @@
         <v>4.5779999999999996E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132" s="11" t="s">
         <v>206</v>
       </c>
@@ -13204,7 +13204,7 @@
         <v>2.4529999999999999E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133" s="11" t="s">
         <v>205</v>
       </c>
@@ -13323,7 +13323,7 @@
         <v>-3.9060000000000002E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134" s="11" t="s">
         <v>204</v>
       </c>
@@ -13442,7 +13442,7 @@
         <v>-8.1899999999999996E-4</v>
       </c>
     </row>
-    <row r="135" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135" s="11" t="s">
         <v>203</v>
       </c>
@@ -13561,7 +13561,7 @@
         <v>1.384E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136" s="11" t="s">
         <v>202</v>
       </c>
@@ -13680,7 +13680,7 @@
         <v>-9.7400000000000004E-4</v>
       </c>
     </row>
-    <row r="137" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137" s="11" t="s">
         <v>201</v>
       </c>
@@ -13799,7 +13799,7 @@
         <v>4.7860000000000003E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138" s="11" t="s">
         <v>200</v>
       </c>
@@ -13918,7 +13918,7 @@
         <v>6.5649999999999997E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139" s="11" t="s">
         <v>199</v>
       </c>
@@ -14037,7 +14037,7 @@
         <v>8.744E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="11" t="s">
         <v>198</v>
       </c>
@@ -14156,145 +14156,145 @@
         <v>4.3969999999999999E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="35" t="s">
+    <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B142" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="C142" s="35"/>
-      <c r="D142" s="35"/>
-      <c r="E142" s="35"/>
-      <c r="F142" s="35"/>
-      <c r="G142" s="35"/>
-      <c r="H142" s="35"/>
-      <c r="I142" s="35"/>
-      <c r="J142" s="35"/>
-      <c r="K142" s="35"/>
-      <c r="L142" s="35"/>
-      <c r="M142" s="35"/>
-      <c r="N142" s="35"/>
-      <c r="O142" s="35"/>
-      <c r="P142" s="35"/>
-      <c r="Q142" s="35"/>
-      <c r="R142" s="35"/>
-      <c r="S142" s="35"/>
-      <c r="T142" s="35"/>
-      <c r="U142" s="35"/>
-      <c r="V142" s="35"/>
-      <c r="W142" s="35"/>
-      <c r="X142" s="35"/>
-      <c r="Y142" s="35"/>
-      <c r="Z142" s="35"/>
-      <c r="AA142" s="35"/>
-      <c r="AB142" s="35"/>
-      <c r="AC142" s="35"/>
-      <c r="AD142" s="35"/>
-      <c r="AE142" s="35"/>
-      <c r="AF142" s="35"/>
-      <c r="AG142" s="35"/>
-      <c r="AH142" s="35"/>
-      <c r="AI142" s="35"/>
-      <c r="AJ142" s="35"/>
-      <c r="AK142" s="35"/>
-      <c r="AL142" s="35"/>
-      <c r="AM142" s="35"/>
-    </row>
-    <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+      <c r="E142" s="36"/>
+      <c r="F142" s="36"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="36"/>
+      <c r="I142" s="36"/>
+      <c r="J142" s="36"/>
+      <c r="K142" s="36"/>
+      <c r="L142" s="36"/>
+      <c r="M142" s="36"/>
+      <c r="N142" s="36"/>
+      <c r="O142" s="36"/>
+      <c r="P142" s="36"/>
+      <c r="Q142" s="36"/>
+      <c r="R142" s="36"/>
+      <c r="S142" s="36"/>
+      <c r="T142" s="36"/>
+      <c r="U142" s="36"/>
+      <c r="V142" s="36"/>
+      <c r="W142" s="36"/>
+      <c r="X142" s="36"/>
+      <c r="Y142" s="36"/>
+      <c r="Z142" s="36"/>
+      <c r="AA142" s="36"/>
+      <c r="AB142" s="36"/>
+      <c r="AC142" s="36"/>
+      <c r="AD142" s="36"/>
+      <c r="AE142" s="36"/>
+      <c r="AF142" s="36"/>
+      <c r="AG142" s="36"/>
+      <c r="AH142" s="36"/>
+      <c r="AI142" s="36"/>
+      <c r="AJ142" s="36"/>
+      <c r="AK142" s="36"/>
+      <c r="AL142" s="36"/>
+      <c r="AM142" s="36"/>
+    </row>
+    <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B143" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="144" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B144" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B145" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B146" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B147" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B148" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B149" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B150" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="151" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B151" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B152" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B153" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="154" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B154" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B155" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B156" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B157" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B158" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="159" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B159" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B160" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B161" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B162" s="7" t="s">
         <v>18</v>
       </c>
@@ -14319,14 +14319,14 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="6"/>
+    <col min="1" max="1" width="19.86328125" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="43.59765625" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="8.73046875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="21" t="s">
         <v>181</v>
       </c>
@@ -14439,8 +14439,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="23" t="s">
         <v>180</v>
       </c>
@@ -14451,7 +14451,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="23" t="s">
         <v>178</v>
       </c>
@@ -14464,7 +14464,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="23" t="s">
         <v>175</v>
       </c>
@@ -14475,7 +14475,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="23" t="s">
         <v>173</v>
       </c>
@@ -14486,7 +14486,7 @@
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="11" t="s">
         <v>171</v>
       </c>
@@ -14494,12 +14494,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
         <v>168</v>
       </c>
@@ -14615,7 +14615,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="19" t="s">
         <v>166</v>
       </c>
@@ -14731,18 +14731,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>163</v>
       </c>
@@ -14861,7 +14861,7 @@
         <v>1.0206E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>161</v>
       </c>
@@ -14980,7 +14980,7 @@
         <v>7.5760000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>159</v>
       </c>
@@ -15099,17 +15099,17 @@
         <v>1.0149999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>156</v>
       </c>
@@ -15228,7 +15228,7 @@
         <v>-5.5329999999999997E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>154</v>
       </c>
@@ -15347,7 +15347,7 @@
         <v>-8.9350000000000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>152</v>
       </c>
@@ -15466,17 +15466,17 @@
         <v>-7.2139999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>148</v>
       </c>
@@ -15595,7 +15595,7 @@
         <v>-3.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>147</v>
       </c>
@@ -15714,7 +15714,7 @@
         <v>-2.9450000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>146</v>
       </c>
@@ -15833,7 +15833,7 @@
         <v>-8.2909999999999998E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>145</v>
       </c>
@@ -15952,7 +15952,7 @@
         <v>-1.1093E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>144</v>
       </c>
@@ -16071,7 +16071,7 @@
         <v>-6.5640000000000004E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>143</v>
       </c>
@@ -16190,7 +16190,7 @@
         <v>-1.9772000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>142</v>
       </c>
@@ -16309,7 +16309,7 @@
         <v>-4.35E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>141</v>
       </c>
@@ -16428,7 +16428,7 @@
         <v>-1.0253E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>140</v>
       </c>
@@ -16547,7 +16547,7 @@
         <v>1.6978E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>139</v>
       </c>
@@ -16666,7 +16666,7 @@
         <v>1.7672E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>137</v>
       </c>
@@ -16785,12 +16785,12 @@
         <v>5.1929999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="11" t="s">
         <v>135</v>
       </c>
@@ -16909,7 +16909,7 @@
         <v>-6.9439999999999997E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>134</v>
       </c>
@@ -17028,7 +17028,7 @@
         <v>-1.3974E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
         <v>133</v>
       </c>
@@ -17147,7 +17147,7 @@
         <v>1.438E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="11" t="s">
         <v>132</v>
       </c>
@@ -17266,7 +17266,7 @@
         <v>9.7310000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="11" t="s">
         <v>131</v>
       </c>
@@ -17385,7 +17385,7 @@
         <v>1.7788999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>129</v>
       </c>
@@ -17504,12 +17504,12 @@
         <v>4.705E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="11" t="s">
         <v>127</v>
       </c>
@@ -17628,7 +17628,7 @@
         <v>-1.0187E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="11" t="s">
         <v>126</v>
       </c>
@@ -17747,7 +17747,7 @@
         <v>2.7700000000000001E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="11" t="s">
         <v>125</v>
       </c>
@@ -17866,7 +17866,7 @@
         <v>2.6340000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
         <v>123</v>
       </c>
@@ -17985,7 +17985,7 @@
         <v>-4.4060000000000002E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="11" t="s">
         <v>122</v>
       </c>
@@ -18104,7 +18104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="11" t="s">
         <v>120</v>
       </c>
@@ -18223,12 +18223,12 @@
         <v>5.3270000000000001E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="11" t="s">
         <v>117</v>
       </c>
@@ -18347,7 +18347,7 @@
         <v>-6.8739999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="11" t="s">
         <v>116</v>
       </c>
@@ -18466,7 +18466,7 @@
         <v>-3.385E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="11" t="s">
         <v>115</v>
       </c>
@@ -18585,7 +18585,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="11" t="s">
         <v>114</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v>-1.1093E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="11" t="s">
         <v>113</v>
       </c>
@@ -18823,7 +18823,7 @@
         <v>7.0070000000000002E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="11" t="s">
         <v>112</v>
       </c>
@@ -18942,7 +18942,7 @@
         <v>-1.9772000000000001E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="11" t="s">
         <v>111</v>
       </c>
@@ -19061,7 +19061,7 @@
         <v>-4.35E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="11" t="s">
         <v>110</v>
       </c>
@@ -19180,7 +19180,7 @@
         <v>-1.0253E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="11" t="s">
         <v>109</v>
       </c>
@@ -19299,7 +19299,7 @@
         <v>1.6978E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="11" t="s">
         <v>108</v>
       </c>
@@ -19418,7 +19418,7 @@
         <v>1.5339E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
         <v>107</v>
       </c>
@@ -19537,7 +19537,7 @@
         <v>4.561E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
         <v>105</v>
       </c>
@@ -19656,12 +19656,12 @@
         <v>1.1249999999999999E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="11" t="s">
         <v>102</v>
       </c>
@@ -19780,7 +19780,7 @@
         <v>-6.5789999999999998E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="11" t="s">
         <v>100</v>
       </c>
@@ -19899,7 +19899,7 @@
         <v>-5.6740000000000002E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="11" t="s">
         <v>98</v>
       </c>
@@ -20018,7 +20018,7 @@
         <v>-3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="11" t="s">
         <v>96</v>
       </c>
@@ -20137,7 +20137,7 @@
         <v>-1.3679E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="11" t="s">
         <v>94</v>
       </c>
@@ -20256,7 +20256,7 @@
         <v>2.9090000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="11" t="s">
         <v>92</v>
       </c>
@@ -20375,7 +20375,7 @@
         <v>-2.2335000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="11" t="s">
         <v>90</v>
       </c>
@@ -20494,7 +20494,7 @@
         <v>-3.0479999999999999E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="11" t="s">
         <v>88</v>
       </c>
@@ -20613,7 +20613,7 @@
         <v>-1.2841E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="11" t="s">
         <v>86</v>
       </c>
@@ -20732,7 +20732,7 @@
         <v>1.4319E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="11" t="s">
         <v>84</v>
       </c>
@@ -20851,7 +20851,7 @@
         <v>1.4466E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="11" t="s">
         <v>82</v>
       </c>
@@ -20970,12 +20970,12 @@
         <v>2.8630000000000001E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="11" t="s">
         <v>79</v>
       </c>
@@ -21094,7 +21094,7 @@
         <v>4.3639999999999998E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="11" t="s">
         <v>77</v>
       </c>
@@ -21213,7 +21213,7 @@
         <v>6.2715999999999994E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="11" t="s">
         <v>75</v>
       </c>
@@ -21332,7 +21332,7 @@
         <v>4.8741E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="11" t="s">
         <v>73</v>
       </c>
@@ -21451,12 +21451,12 @@
         <v>4.7280999999999997E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="11" t="s">
         <v>70</v>
       </c>
@@ -21575,7 +21575,7 @@
         <v>-1.8090000000000001E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="11" t="s">
         <v>69</v>
       </c>
@@ -21694,7 +21694,7 @@
         <v>-1.7240000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="11" t="s">
         <v>68</v>
       </c>
@@ -21813,7 +21813,7 @@
         <v>1.0460000000000001E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="11" t="s">
         <v>67</v>
       </c>
@@ -21932,7 +21932,7 @@
         <v>1.934E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="11" t="s">
         <v>66</v>
       </c>
@@ -22051,7 +22051,7 @@
         <v>-2.6310000000000001E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="11" t="s">
         <v>65</v>
       </c>
@@ -22170,7 +22170,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="11" t="s">
         <v>64</v>
       </c>
@@ -22289,7 +22289,7 @@
         <v>1.5E-5</v>
       </c>
     </row>
-    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="11" t="s">
         <v>63</v>
       </c>
@@ -22408,7 +22408,7 @@
         <v>-9.4700000000000003E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="11" t="s">
         <v>62</v>
       </c>
@@ -22527,7 +22527,7 @@
         <v>1.7769999999999999E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="11" t="s">
         <v>61</v>
       </c>
@@ -22646,12 +22646,12 @@
         <v>-1.3990000000000001E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="11" t="s">
         <v>59</v>
       </c>
@@ -22770,7 +22770,7 @@
         <v>4.5779999999999996E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="11" t="s">
         <v>57</v>
       </c>
@@ -22889,7 +22889,7 @@
         <v>2.4529999999999999E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="11" t="s">
         <v>55</v>
       </c>
@@ -23008,7 +23008,7 @@
         <v>-3.9060000000000002E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="11" t="s">
         <v>53</v>
       </c>
@@ -23127,7 +23127,7 @@
         <v>-8.1899999999999996E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="11" t="s">
         <v>51</v>
       </c>
@@ -23246,7 +23246,7 @@
         <v>1.384E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
@@ -23365,7 +23365,7 @@
         <v>-9.7400000000000004E-4</v>
       </c>
     </row>
-    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="11" t="s">
         <v>47</v>
       </c>
@@ -23484,7 +23484,7 @@
         <v>4.7860000000000003E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="11" t="s">
         <v>45</v>
       </c>
@@ -23603,7 +23603,7 @@
         <v>6.5649999999999997E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="11" t="s">
         <v>43</v>
       </c>
@@ -23722,7 +23722,7 @@
         <v>8.744E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="11" t="s">
         <v>41</v>
       </c>
@@ -23841,150 +23841,150 @@
         <v>4.3969999999999999E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="35" t="s">
+    <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B118" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="35"/>
-      <c r="H118" s="35"/>
-      <c r="I118" s="35"/>
-      <c r="J118" s="35"/>
-      <c r="K118" s="35"/>
-      <c r="L118" s="35"/>
-      <c r="M118" s="35"/>
-      <c r="N118" s="35"/>
-      <c r="O118" s="35"/>
-      <c r="P118" s="35"/>
-      <c r="Q118" s="35"/>
-      <c r="R118" s="35"/>
-      <c r="S118" s="35"/>
-      <c r="T118" s="35"/>
-      <c r="U118" s="35"/>
-      <c r="V118" s="35"/>
-      <c r="W118" s="35"/>
-      <c r="X118" s="35"/>
-      <c r="Y118" s="35"/>
-      <c r="Z118" s="35"/>
-      <c r="AA118" s="35"/>
-      <c r="AB118" s="35"/>
-      <c r="AC118" s="35"/>
-      <c r="AD118" s="35"/>
-      <c r="AE118" s="35"/>
-      <c r="AF118" s="35"/>
-      <c r="AG118" s="35"/>
-      <c r="AH118" s="35"/>
-      <c r="AI118" s="35"/>
-      <c r="AJ118" s="35"/>
-      <c r="AK118" s="35"/>
-      <c r="AL118" s="35"/>
-      <c r="AM118" s="35"/>
-    </row>
-    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="36"/>
+      <c r="G118" s="36"/>
+      <c r="H118" s="36"/>
+      <c r="I118" s="36"/>
+      <c r="J118" s="36"/>
+      <c r="K118" s="36"/>
+      <c r="L118" s="36"/>
+      <c r="M118" s="36"/>
+      <c r="N118" s="36"/>
+      <c r="O118" s="36"/>
+      <c r="P118" s="36"/>
+      <c r="Q118" s="36"/>
+      <c r="R118" s="36"/>
+      <c r="S118" s="36"/>
+      <c r="T118" s="36"/>
+      <c r="U118" s="36"/>
+      <c r="V118" s="36"/>
+      <c r="W118" s="36"/>
+      <c r="X118" s="36"/>
+      <c r="Y118" s="36"/>
+      <c r="Z118" s="36"/>
+      <c r="AA118" s="36"/>
+      <c r="AB118" s="36"/>
+      <c r="AC118" s="36"/>
+      <c r="AD118" s="36"/>
+      <c r="AE118" s="36"/>
+      <c r="AF118" s="36"/>
+      <c r="AG118" s="36"/>
+      <c r="AH118" s="36"/>
+      <c r="AI118" s="36"/>
+      <c r="AJ118" s="36"/>
+      <c r="AK118" s="36"/>
+      <c r="AL118" s="36"/>
+      <c r="AM118" s="36"/>
+    </row>
+    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B119" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B121" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B122" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B123" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B124" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B125" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B126" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B127" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B128" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B129" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B130" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="131" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B131" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B132" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B133" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B134" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B135" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B136" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B137" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B138" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B139" s="7" t="s">
         <v>18</v>
       </c>
@@ -24004,21 +24004,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A1" s="30" t="s">
         <v>182</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="B2">
         <v>2015</v>
       </c>
@@ -24128,7 +24128,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>345</v>
       </c>
@@ -24277,7 +24277,7 @@
         <v>2.0387429639167166E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -24286,19 +24286,19 @@
         <v>2.1866115765726366E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A8" s="30" t="s">
         <v>184</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
       <c r="B12" s="27" t="s">
         <v>344</v>
       </c>
@@ -24306,7 +24306,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>340</v>
       </c>
@@ -24314,7 +24314,7 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>341</v>
       </c>
@@ -24322,7 +24322,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>342</v>
       </c>
@@ -24330,12 +24330,12 @@
         <v>0.96599999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>2015</v>
       </c>
@@ -24445,7 +24445,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>340</v>
       </c>
@@ -24590,7 +24590,7 @@
         <v>106.80688818099999</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>341</v>
       </c>
@@ -24735,7 +24735,7 @@
         <v>40.991097584999999</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>342</v>
       </c>
@@ -24880,12 +24880,12 @@
         <v>4.4407329119999996</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>2015</v>
       </c>
@@ -24995,7 +24995,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>340</v>
       </c>
@@ -25140,7 +25140,7 @@
         <v>1.1215938190000116</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>341</v>
       </c>
@@ -25285,7 +25285,7 @@
         <v>0.52974641499999819</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>342</v>
       </c>
@@ -25430,12 +25430,12 @@
         <v>0.12269708800000068</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>2015</v>
       </c>
@@ -25545,7 +25545,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>340</v>
       </c>
@@ -25690,7 +25690,7 @@
         <v>1.0501137502473678E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>341</v>
       </c>
@@ -25835,7 +25835,7 @@
         <v>1.2923450363862663E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>342</v>
       </c>
@@ -25980,15 +25980,15 @@
         <v>2.7629918401181404E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.45">
       <c r="C34" s="25"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>340</v>
       </c>
@@ -25997,7 +25997,7 @@
         <v>1.143000484613816E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>341</v>
       </c>
@@ -26006,7 +26006,7 @@
         <v>1.5514513735396921E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>342</v>
       </c>
@@ -26015,12 +26015,12 @@
         <v>2.7312273593190856E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>352</v>
       </c>
@@ -26029,34 +26029,34 @@
         <v>1.3254110935573082E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A44" s="30" t="s">
         <v>356</v>
       </c>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>361</v>
       </c>
@@ -26065,7 +26065,7 @@
         <v>0.97813388423427361</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>362</v>
       </c>
@@ -26074,12 +26074,12 @@
         <v>0.98674588906442695</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -26088,7 +26088,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -26097,7 +26097,7 @@
         <v>6.3157894736842107E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -26106,7 +26106,7 @@
         <v>0.1095</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -26115,7 +26115,7 @@
         <v>7.3891625615763554E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -26124,12 +26124,12 @@
         <v>6.4935064935064929E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
         <v>361</v>
       </c>
@@ -26137,7 +26137,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -26150,7 +26150,7 @@
         <v>6.5188105096858712E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -26163,7 +26163,7 @@
         <v>7.5574903929115839E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -26176,7 +26176,7 @@
         <v>0.12130278578812782</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -26189,7 +26189,7 @@
         <v>8.6166368748215469E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -26214,15 +26214,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.73046875" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B1" s="27" t="s">
         <v>353</v>
       </c>
@@ -26233,7 +26233,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -26250,7 +26250,7 @@
         <v>7.3346846514898659E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -26267,7 +26267,7 @@
         <v>8.3642992664733129E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -26281,7 +26281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -26298,7 +26298,7 @@
         <v>0.12897177608937932</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -26315,7 +26315,7 @@
         <v>9.4142018541657921E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -26332,7 +26332,7 @@
         <v>8.5381303053666202E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D8" s="4"/>
     </row>
   </sheetData>
@@ -26347,18 +26347,20 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.73046875" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="35" t="s">
         <v>381</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -26371,37 +26373,37 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>4.5699999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C2" s="4">
         <f>B2</f>
-        <v>4.5699999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D2" s="34">
-        <v>4.7800000000000002E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="34">
-        <v>5.7000000000000002E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="C3" s="4">
         <f>B3</f>
-        <v>5.7000000000000002E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D3" s="34">
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -26415,7 +26417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -26430,7 +26432,7 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -26445,22 +26447,22 @@
         <v>7.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="34">
-        <v>6.7500000000000004E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="C7" s="4">
         <f>B7</f>
-        <v>6.7500000000000004E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="D7" s="34">
-        <v>6.9500000000000006E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.3500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D8" s="4"/>
     </row>
   </sheetData>

</xml_diff>